<commit_message>
Completed all 100,1000, 10000, 100000 iteration pages with durations, and added the durations to the TimeDuration excel file.  Next will be charting the differences on a TimeDuration page, to show the duration timing differences between LinkedLists, Binary Trees, and Hash Tables.
</commit_message>
<xml_diff>
--- a/MyHashTable100_000.xlsx
+++ b/MyHashTable100_000.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hachidori\PycharmProjects\HashTableProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C44C897D-1EF5-445F-A21C-678689E2B4B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{970511BF-A97B-4AAD-85FE-2D0080D68586}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{362F65DA-2CCB-4A7D-87E0-21DEA51A8ADE}"/>
+    <workbookView xWindow="-13515" yWindow="0" windowWidth="11025" windowHeight="10800" xr2:uid="{A3B4944D-2233-45F5-B70E-BA5EE655FF74}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -378,7 +378,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E540C166-D07A-4BEF-9F97-0B9E4014AA84}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D63995-9413-436A-8C63-A2C7FE31B5CC}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>